<commit_message>
title, dynamical description and answers from db
</commit_message>
<xml_diff>
--- a/data/Devine-voir_words.xlsx
+++ b/data/Devine-voir_words.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yemer\Dropbox\Dis-voir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FREELANCE PROJECT\CLIENTS\Richman\wordle-game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276004B2-70E7-4169-9E10-4B098DEE9C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BC5DAF53-4B63-4D6A-8B7C-74E6FE683706}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$E$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -208,8 +207,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -580,16 +579,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DABED74-2F95-4F3A-92F3-7E4C205FAA20}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -606,7 +605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -620,7 +619,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -634,7 +633,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -648,7 +647,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -662,7 +661,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -676,7 +675,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -690,7 +689,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -704,7 +703,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -718,7 +717,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -732,7 +731,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -746,7 +745,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -761,7 +760,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{1DABED74-2F95-4F3A-92F3-7E4C205FAA20}"/>
+  <autoFilter ref="A1:E1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>